<commit_message>
update for project events and rearrange folders
</commit_message>
<xml_diff>
--- a/Capex/raw_data/Concordance-Tables-Capex.xlsx
+++ b/Capex/raw_data/Concordance-Tables-Capex.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iimv1-my.sharepoint.com/personal/kalyan_iimv_ac_in/Documents/Python-Exercise-KK/Kalyan-Jupyter-Notebooks/Capex/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{A4298C09-4619-D04D-A8C0-7D5F69C903D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D2BD9C1-2E5D-2148-A57A-B2D3F1A307A7}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{A4298C09-4619-D04D-A8C0-7D5F69C903D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8808FC26-2613-5E47-87BF-75E3EE2F446E}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14600" xr2:uid="{066F22B7-05DB-8447-9D9F-075A965A6F91}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14600" activeTab="2" xr2:uid="{066F22B7-05DB-8447-9D9F-075A965A6F91}"/>
   </bookViews>
   <sheets>
     <sheet name="state-concord" sheetId="1" r:id="rId1"/>
     <sheet name="ind-concord" sheetId="3" r:id="rId2"/>
+    <sheet name="events-concord" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="549">
   <si>
     <t>Andaman &amp; Nicobar Islands</t>
   </si>
@@ -922,6 +923,768 @@
   </si>
   <si>
     <t>IndG</t>
+  </si>
+  <si>
+    <t>Transferred from</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Transferred to</t>
+  </si>
+  <si>
+    <t>Issues resolved by CCI</t>
+  </si>
+  <si>
+    <t>Project cost</t>
+  </si>
+  <si>
+    <t>Expenditure incurred till</t>
+  </si>
+  <si>
+    <t>Company contacted but no response</t>
+  </si>
+  <si>
+    <t>Company contacted successfully</t>
+  </si>
+  <si>
+    <t>De-notification request approved by BoA/SEZ Board</t>
+  </si>
+  <si>
+    <t>End Stage</t>
+  </si>
+  <si>
+    <t>End stages of completion or of shelving</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>PPA cancelled</t>
+  </si>
+  <si>
+    <t>Formal approval cancelled by SEZ Board (BoA)</t>
+  </si>
+  <si>
+    <t>Rejected by SEZ Board</t>
+  </si>
+  <si>
+    <t>No information upto</t>
+  </si>
+  <si>
+    <t>Rejected by Govt.</t>
+  </si>
+  <si>
+    <t>No information</t>
+  </si>
+  <si>
+    <t>Stalled upto</t>
+  </si>
+  <si>
+    <t>Shelved on</t>
+  </si>
+  <si>
+    <t>Stalled on</t>
+  </si>
+  <si>
+    <t>Implementation stalled on</t>
+  </si>
+  <si>
+    <t>Abandoned on</t>
+  </si>
+  <si>
+    <t>Commercial production commenced</t>
+  </si>
+  <si>
+    <t>Completion By - Estd. By CMIE For Product/unit</t>
+  </si>
+  <si>
+    <t>Commercial production commenced For Product/unit</t>
+  </si>
+  <si>
+    <t>Comm. Prod Expected</t>
+  </si>
+  <si>
+    <t>Completed For Product/unit</t>
+  </si>
+  <si>
+    <t>Completion By</t>
+  </si>
+  <si>
+    <t>Completion By - Estd. By CMIE</t>
+  </si>
+  <si>
+    <t>Comm. Prod Expected For Product/unit</t>
+  </si>
+  <si>
+    <t>Completion By For Product/unit</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Initial Commissioning Date</t>
+  </si>
+  <si>
+    <t>Initial Commissioning Date - Estd. By CMIE</t>
+  </si>
+  <si>
+    <t>Initial Commissioning Date - Estd. By CMIE For Product/unit</t>
+  </si>
+  <si>
+    <t>Initial Commissioning Date For Product/unit</t>
+  </si>
+  <si>
+    <t>Partially commissioned</t>
+  </si>
+  <si>
+    <t>Partially commissioned by</t>
+  </si>
+  <si>
+    <t>Trial run commenced</t>
+  </si>
+  <si>
+    <t>Trial run expected</t>
+  </si>
+  <si>
+    <t>Physical progress</t>
+  </si>
+  <si>
+    <t>Ongoing Construction</t>
+  </si>
+  <si>
+    <t>The stage of construction - both civil and machinery</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Construction completed</t>
+  </si>
+  <si>
+    <t>Construction completion expected</t>
+  </si>
+  <si>
+    <t>Construction commenced</t>
+  </si>
+  <si>
+    <t>Construction commencement expected</t>
+  </si>
+  <si>
+    <t>Machinery installed</t>
+  </si>
+  <si>
+    <t>Foundation stone laid</t>
+  </si>
+  <si>
+    <t>Machinery ordered</t>
+  </si>
+  <si>
+    <t>Implementation started</t>
+  </si>
+  <si>
+    <t>Land allotment cancelled</t>
+  </si>
+  <si>
+    <t>Seek Land</t>
+  </si>
+  <si>
+    <t>Stage consisting of bidding, negotiating and buying land</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Land acquired returned</t>
+  </si>
+  <si>
+    <t>Land acquired</t>
+  </si>
+  <si>
+    <t>Land acquisition problem resolved</t>
+  </si>
+  <si>
+    <t>Land acquisition problem</t>
+  </si>
+  <si>
+    <t>Land acquisition awaited</t>
+  </si>
+  <si>
+    <t>Offer for sale raised</t>
+  </si>
+  <si>
+    <t>Receipt Financial Closure</t>
+  </si>
+  <si>
+    <t>The stage when funds are sought or when financial closure is achieved</t>
+  </si>
+  <si>
+    <t>Financial closure achieved</t>
+  </si>
+  <si>
+    <t>Equity/Debenture issue raised</t>
+  </si>
+  <si>
+    <t>Loan sanctioned</t>
+  </si>
+  <si>
+    <t>Funds not tied-up</t>
+  </si>
+  <si>
+    <t>OTCEI issue raised</t>
+  </si>
+  <si>
+    <t>Budgetary allocation</t>
+  </si>
+  <si>
+    <t>Contract mode changed</t>
+  </si>
+  <si>
+    <t>Seek Bids</t>
+  </si>
+  <si>
+    <t>The stage when the project invites bids from implementors</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Contract cancelled</t>
+  </si>
+  <si>
+    <t>Bids awarded</t>
+  </si>
+  <si>
+    <t>Bids cancelled</t>
+  </si>
+  <si>
+    <t>Bids opening deferred</t>
+  </si>
+  <si>
+    <t>Consultants appointed</t>
+  </si>
+  <si>
+    <t>Bids invited</t>
+  </si>
+  <si>
+    <t>Contract termination revoked</t>
+  </si>
+  <si>
+    <t>FAC recommendation received</t>
+  </si>
+  <si>
+    <t>Receipt Approvals</t>
+  </si>
+  <si>
+    <t>The stage when the initial approvals have been received</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>EAC recommendation received</t>
+  </si>
+  <si>
+    <t>CRZ clearance received</t>
+  </si>
+  <si>
+    <t>FC received</t>
+  </si>
+  <si>
+    <t>MRTP clearance received</t>
+  </si>
+  <si>
+    <t>Fuel Supply Agreement (FSA) signed</t>
+  </si>
+  <si>
+    <t>Power supply sanctioned</t>
+  </si>
+  <si>
+    <t>PPA signed</t>
+  </si>
+  <si>
+    <t>Coal linkage granted</t>
+  </si>
+  <si>
+    <t>CEA in-principle appr received</t>
+  </si>
+  <si>
+    <t>CEA initial approval received</t>
+  </si>
+  <si>
+    <t>CCFI approval received</t>
+  </si>
+  <si>
+    <t>CCEA approval received</t>
+  </si>
+  <si>
+    <t>PIB approval received</t>
+  </si>
+  <si>
+    <t>SEZ Board In-principle appr Received</t>
+  </si>
+  <si>
+    <t>SEZ Board formal approval received</t>
+  </si>
+  <si>
+    <t>SEZ Board notified</t>
+  </si>
+  <si>
+    <t>SIA clearance received</t>
+  </si>
+  <si>
+    <t>Environmental clearance received</t>
+  </si>
+  <si>
+    <t>Approved by Planning Commission</t>
+  </si>
+  <si>
+    <t>Cabinet approval received</t>
+  </si>
+  <si>
+    <t>State Govt approval received</t>
+  </si>
+  <si>
+    <t>Central Govt approval received</t>
+  </si>
+  <si>
+    <t>Letter of Intent (LoI) received</t>
+  </si>
+  <si>
+    <t>Licence received</t>
+  </si>
+  <si>
+    <t>MRTP clearance sought</t>
+  </si>
+  <si>
+    <t>Seek Approvals</t>
+  </si>
+  <si>
+    <t>The stage of seeking initial approvals</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Coal linkage sought</t>
+  </si>
+  <si>
+    <t>CEA approval sought</t>
+  </si>
+  <si>
+    <t>FIPB approval received</t>
+  </si>
+  <si>
+    <t>Forest clearance sought</t>
+  </si>
+  <si>
+    <t>Environment clearance sought</t>
+  </si>
+  <si>
+    <t>State Govt. approval sought</t>
+  </si>
+  <si>
+    <t>Central Govt. approval sought</t>
+  </si>
+  <si>
+    <t>Letter of Intent (LoI) sought</t>
+  </si>
+  <si>
+    <t>Licence agreement signed</t>
+  </si>
+  <si>
+    <t>Licence sought</t>
+  </si>
+  <si>
+    <t>Feasibility report prepared</t>
+  </si>
+  <si>
+    <t>MoU cancelled</t>
+  </si>
+  <si>
+    <t>Collaboration approved</t>
+  </si>
+  <si>
+    <t>Announcement</t>
+  </si>
+  <si>
+    <t>Initial stages of announcement</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>BoD approval received</t>
+  </si>
+  <si>
+    <t>Co-promoters Invited</t>
+  </si>
+  <si>
+    <t>IEM filed</t>
+  </si>
+  <si>
+    <t>MoU signed</t>
+  </si>
+  <si>
+    <t>sub_stage_id</t>
+  </si>
+  <si>
+    <t>stage_desc_short</t>
+  </si>
+  <si>
+    <t>stage_desc_long</t>
+  </si>
+  <si>
+    <t>stage_id</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>sub_stage_sno</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>H11</t>
+  </si>
+  <si>
+    <t>H12</t>
+  </si>
+  <si>
+    <t>H13</t>
+  </si>
+  <si>
+    <t>H14</t>
+  </si>
+  <si>
+    <t>H15</t>
+  </si>
+  <si>
+    <t>H16</t>
+  </si>
+  <si>
+    <t>H17</t>
+  </si>
+  <si>
+    <t>H18</t>
+  </si>
+  <si>
+    <t>H19</t>
+  </si>
+  <si>
+    <t>H20</t>
+  </si>
+  <si>
+    <t>H21</t>
+  </si>
+  <si>
+    <t>H22</t>
+  </si>
+  <si>
+    <t>H23</t>
+  </si>
+  <si>
+    <t>H24</t>
+  </si>
+  <si>
+    <t>H25</t>
+  </si>
+  <si>
+    <t>H26</t>
+  </si>
+  <si>
+    <t>H27</t>
+  </si>
+  <si>
+    <t>H28</t>
+  </si>
+  <si>
+    <t>H29</t>
+  </si>
+  <si>
+    <t>H30</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>I6</t>
+  </si>
+  <si>
+    <t>I7</t>
+  </si>
+  <si>
+    <t>parent_sub_stage_id</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +2069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE6C8A3-DE9F-6A43-A0A0-F398A00B4536}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2909,4 +3672,2269 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF3662F-482F-C043-A2BE-B88B35FEFF90}">
+  <dimension ref="A1:G112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>438</v>
+      </c>
+      <c r="F3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>439</v>
+      </c>
+      <c r="F4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>440</v>
+      </c>
+      <c r="F5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>426</v>
+      </c>
+      <c r="B6" t="s">
+        <v>425</v>
+      </c>
+      <c r="C6" t="s">
+        <v>424</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>441</v>
+      </c>
+      <c r="F6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>426</v>
+      </c>
+      <c r="B7" t="s">
+        <v>425</v>
+      </c>
+      <c r="C7" t="s">
+        <v>424</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>442</v>
+      </c>
+      <c r="F7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B8" t="s">
+        <v>409</v>
+      </c>
+      <c r="C8" t="s">
+        <v>408</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>443</v>
+      </c>
+      <c r="F8" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" t="s">
+        <v>409</v>
+      </c>
+      <c r="C9" t="s">
+        <v>408</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>444</v>
+      </c>
+      <c r="F9" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>410</v>
+      </c>
+      <c r="B10" t="s">
+        <v>409</v>
+      </c>
+      <c r="C10" t="s">
+        <v>408</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>445</v>
+      </c>
+      <c r="F10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>410</v>
+      </c>
+      <c r="B11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C11" t="s">
+        <v>408</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>446</v>
+      </c>
+      <c r="F11" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>410</v>
+      </c>
+      <c r="B12" t="s">
+        <v>409</v>
+      </c>
+      <c r="C12" t="s">
+        <v>408</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>447</v>
+      </c>
+      <c r="F12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" t="s">
+        <v>409</v>
+      </c>
+      <c r="C13" t="s">
+        <v>408</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>448</v>
+      </c>
+      <c r="F13" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>410</v>
+      </c>
+      <c r="B14" t="s">
+        <v>409</v>
+      </c>
+      <c r="C14" t="s">
+        <v>408</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>449</v>
+      </c>
+      <c r="F14" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>410</v>
+      </c>
+      <c r="B15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C15" t="s">
+        <v>408</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>450</v>
+      </c>
+      <c r="F15" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B16" t="s">
+        <v>409</v>
+      </c>
+      <c r="C16" t="s">
+        <v>408</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>451</v>
+      </c>
+      <c r="F16" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>410</v>
+      </c>
+      <c r="B17" t="s">
+        <v>409</v>
+      </c>
+      <c r="C17" t="s">
+        <v>408</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>452</v>
+      </c>
+      <c r="F17" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>410</v>
+      </c>
+      <c r="B18" t="s">
+        <v>409</v>
+      </c>
+      <c r="C18" t="s">
+        <v>408</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>453</v>
+      </c>
+      <c r="F18" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>410</v>
+      </c>
+      <c r="B19" t="s">
+        <v>409</v>
+      </c>
+      <c r="C19" t="s">
+        <v>408</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>454</v>
+      </c>
+      <c r="F19" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>410</v>
+      </c>
+      <c r="B20" t="s">
+        <v>409</v>
+      </c>
+      <c r="C20" t="s">
+        <v>408</v>
+      </c>
+      <c r="D20">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>455</v>
+      </c>
+      <c r="F20" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>382</v>
+      </c>
+      <c r="B21" t="s">
+        <v>381</v>
+      </c>
+      <c r="C21" t="s">
+        <v>380</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>456</v>
+      </c>
+      <c r="F21" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>382</v>
+      </c>
+      <c r="B22" t="s">
+        <v>381</v>
+      </c>
+      <c r="C22" t="s">
+        <v>380</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>457</v>
+      </c>
+      <c r="F22" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>382</v>
+      </c>
+      <c r="B23" t="s">
+        <v>381</v>
+      </c>
+      <c r="C23" t="s">
+        <v>380</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>458</v>
+      </c>
+      <c r="F23" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>382</v>
+      </c>
+      <c r="B24" t="s">
+        <v>381</v>
+      </c>
+      <c r="C24" t="s">
+        <v>380</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>459</v>
+      </c>
+      <c r="F24" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>382</v>
+      </c>
+      <c r="B25" t="s">
+        <v>381</v>
+      </c>
+      <c r="C25" t="s">
+        <v>380</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>460</v>
+      </c>
+      <c r="F25" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" t="s">
+        <v>381</v>
+      </c>
+      <c r="C26" t="s">
+        <v>380</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>461</v>
+      </c>
+      <c r="F26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>382</v>
+      </c>
+      <c r="B27" t="s">
+        <v>381</v>
+      </c>
+      <c r="C27" t="s">
+        <v>380</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>462</v>
+      </c>
+      <c r="F27" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>382</v>
+      </c>
+      <c r="B28" t="s">
+        <v>381</v>
+      </c>
+      <c r="C28" t="s">
+        <v>380</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>463</v>
+      </c>
+      <c r="F28" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>382</v>
+      </c>
+      <c r="B29" t="s">
+        <v>381</v>
+      </c>
+      <c r="C29" t="s">
+        <v>380</v>
+      </c>
+      <c r="D29">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>464</v>
+      </c>
+      <c r="F29" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>382</v>
+      </c>
+      <c r="B30" t="s">
+        <v>381</v>
+      </c>
+      <c r="C30" t="s">
+        <v>380</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>465</v>
+      </c>
+      <c r="F30" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>382</v>
+      </c>
+      <c r="B31" t="s">
+        <v>381</v>
+      </c>
+      <c r="C31" t="s">
+        <v>380</v>
+      </c>
+      <c r="D31">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>466</v>
+      </c>
+      <c r="F31" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>382</v>
+      </c>
+      <c r="B32" t="s">
+        <v>381</v>
+      </c>
+      <c r="C32" t="s">
+        <v>380</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>467</v>
+      </c>
+      <c r="F32" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>382</v>
+      </c>
+      <c r="B33" t="s">
+        <v>381</v>
+      </c>
+      <c r="C33" t="s">
+        <v>380</v>
+      </c>
+      <c r="D33">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>468</v>
+      </c>
+      <c r="F33" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>382</v>
+      </c>
+      <c r="B34" t="s">
+        <v>381</v>
+      </c>
+      <c r="C34" t="s">
+        <v>380</v>
+      </c>
+      <c r="D34">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>469</v>
+      </c>
+      <c r="F34" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>382</v>
+      </c>
+      <c r="B35" t="s">
+        <v>381</v>
+      </c>
+      <c r="C35" t="s">
+        <v>380</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>470</v>
+      </c>
+      <c r="F35" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>382</v>
+      </c>
+      <c r="B36" t="s">
+        <v>381</v>
+      </c>
+      <c r="C36" t="s">
+        <v>380</v>
+      </c>
+      <c r="D36">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>471</v>
+      </c>
+      <c r="F36" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>382</v>
+      </c>
+      <c r="B37" t="s">
+        <v>381</v>
+      </c>
+      <c r="C37" t="s">
+        <v>380</v>
+      </c>
+      <c r="D37">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>472</v>
+      </c>
+      <c r="F37" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>382</v>
+      </c>
+      <c r="B38" t="s">
+        <v>381</v>
+      </c>
+      <c r="C38" t="s">
+        <v>380</v>
+      </c>
+      <c r="D38">
+        <v>18</v>
+      </c>
+      <c r="E38" t="s">
+        <v>473</v>
+      </c>
+      <c r="F38" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>382</v>
+      </c>
+      <c r="B39" t="s">
+        <v>381</v>
+      </c>
+      <c r="C39" t="s">
+        <v>380</v>
+      </c>
+      <c r="D39">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>474</v>
+      </c>
+      <c r="F39" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>382</v>
+      </c>
+      <c r="B40" t="s">
+        <v>381</v>
+      </c>
+      <c r="C40" t="s">
+        <v>380</v>
+      </c>
+      <c r="D40">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>475</v>
+      </c>
+      <c r="F40" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>382</v>
+      </c>
+      <c r="B41" t="s">
+        <v>381</v>
+      </c>
+      <c r="C41" t="s">
+        <v>380</v>
+      </c>
+      <c r="D41">
+        <v>21</v>
+      </c>
+      <c r="E41" t="s">
+        <v>476</v>
+      </c>
+      <c r="F41" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>382</v>
+      </c>
+      <c r="B42" t="s">
+        <v>381</v>
+      </c>
+      <c r="C42" t="s">
+        <v>380</v>
+      </c>
+      <c r="D42">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>477</v>
+      </c>
+      <c r="F42" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>382</v>
+      </c>
+      <c r="B43" t="s">
+        <v>381</v>
+      </c>
+      <c r="C43" t="s">
+        <v>380</v>
+      </c>
+      <c r="D43">
+        <v>23</v>
+      </c>
+      <c r="E43" t="s">
+        <v>478</v>
+      </c>
+      <c r="F43" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>382</v>
+      </c>
+      <c r="B44" t="s">
+        <v>381</v>
+      </c>
+      <c r="C44" t="s">
+        <v>380</v>
+      </c>
+      <c r="D44">
+        <v>24</v>
+      </c>
+      <c r="E44" t="s">
+        <v>479</v>
+      </c>
+      <c r="F44" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>382</v>
+      </c>
+      <c r="B45" t="s">
+        <v>381</v>
+      </c>
+      <c r="C45" t="s">
+        <v>380</v>
+      </c>
+      <c r="D45">
+        <v>25</v>
+      </c>
+      <c r="E45" t="s">
+        <v>480</v>
+      </c>
+      <c r="F45" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>371</v>
+      </c>
+      <c r="B46" t="s">
+        <v>370</v>
+      </c>
+      <c r="C46" t="s">
+        <v>369</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>481</v>
+      </c>
+      <c r="F46" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>371</v>
+      </c>
+      <c r="B47" t="s">
+        <v>370</v>
+      </c>
+      <c r="C47" t="s">
+        <v>369</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>482</v>
+      </c>
+      <c r="F47" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>371</v>
+      </c>
+      <c r="B48" t="s">
+        <v>370</v>
+      </c>
+      <c r="C48" t="s">
+        <v>369</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>483</v>
+      </c>
+      <c r="F48" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>371</v>
+      </c>
+      <c r="B49" t="s">
+        <v>370</v>
+      </c>
+      <c r="C49" t="s">
+        <v>369</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>484</v>
+      </c>
+      <c r="F49" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>371</v>
+      </c>
+      <c r="B50" t="s">
+        <v>370</v>
+      </c>
+      <c r="C50" t="s">
+        <v>369</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>485</v>
+      </c>
+      <c r="F50" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>371</v>
+      </c>
+      <c r="B51" t="s">
+        <v>370</v>
+      </c>
+      <c r="C51" t="s">
+        <v>369</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>486</v>
+      </c>
+      <c r="F51" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>371</v>
+      </c>
+      <c r="B52" t="s">
+        <v>370</v>
+      </c>
+      <c r="C52" t="s">
+        <v>369</v>
+      </c>
+      <c r="D52">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>487</v>
+      </c>
+      <c r="F52" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>371</v>
+      </c>
+      <c r="B53" t="s">
+        <v>370</v>
+      </c>
+      <c r="C53" t="s">
+        <v>369</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>488</v>
+      </c>
+      <c r="F53" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" t="s">
+        <v>361</v>
+      </c>
+      <c r="C54" t="s">
+        <v>360</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>489</v>
+      </c>
+      <c r="F54" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" t="s">
+        <v>361</v>
+      </c>
+      <c r="C55" t="s">
+        <v>360</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>490</v>
+      </c>
+      <c r="F55" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" t="s">
+        <v>361</v>
+      </c>
+      <c r="C56" t="s">
+        <v>360</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>491</v>
+      </c>
+      <c r="F56" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" t="s">
+        <v>361</v>
+      </c>
+      <c r="C57" t="s">
+        <v>360</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>492</v>
+      </c>
+      <c r="F57" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" t="s">
+        <v>361</v>
+      </c>
+      <c r="C58" t="s">
+        <v>360</v>
+      </c>
+      <c r="D58">
+        <v>5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>493</v>
+      </c>
+      <c r="F58" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" t="s">
+        <v>361</v>
+      </c>
+      <c r="C59" t="s">
+        <v>360</v>
+      </c>
+      <c r="D59">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>494</v>
+      </c>
+      <c r="F59" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" t="s">
+        <v>361</v>
+      </c>
+      <c r="C60" t="s">
+        <v>360</v>
+      </c>
+      <c r="D60">
+        <v>7</v>
+      </c>
+      <c r="E60" t="s">
+        <v>495</v>
+      </c>
+      <c r="F60" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>353</v>
+      </c>
+      <c r="B61" t="s">
+        <v>352</v>
+      </c>
+      <c r="C61" t="s">
+        <v>351</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>496</v>
+      </c>
+      <c r="F61" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>353</v>
+      </c>
+      <c r="B62" t="s">
+        <v>352</v>
+      </c>
+      <c r="C62" t="s">
+        <v>351</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62" t="s">
+        <v>497</v>
+      </c>
+      <c r="F62" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>353</v>
+      </c>
+      <c r="B63" t="s">
+        <v>352</v>
+      </c>
+      <c r="C63" t="s">
+        <v>351</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>498</v>
+      </c>
+      <c r="F63" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>353</v>
+      </c>
+      <c r="B64" t="s">
+        <v>352</v>
+      </c>
+      <c r="C64" t="s">
+        <v>351</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="E64" t="s">
+        <v>499</v>
+      </c>
+      <c r="F64" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>353</v>
+      </c>
+      <c r="B65" t="s">
+        <v>352</v>
+      </c>
+      <c r="C65" t="s">
+        <v>351</v>
+      </c>
+      <c r="D65">
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>500</v>
+      </c>
+      <c r="F65" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>353</v>
+      </c>
+      <c r="B66" t="s">
+        <v>352</v>
+      </c>
+      <c r="C66" t="s">
+        <v>351</v>
+      </c>
+      <c r="D66">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>501</v>
+      </c>
+      <c r="F66" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>341</v>
+      </c>
+      <c r="B67" t="s">
+        <v>340</v>
+      </c>
+      <c r="C67" t="s">
+        <v>339</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>502</v>
+      </c>
+      <c r="F67" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>341</v>
+      </c>
+      <c r="B68" t="s">
+        <v>340</v>
+      </c>
+      <c r="C68" t="s">
+        <v>339</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>503</v>
+      </c>
+      <c r="F68" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>341</v>
+      </c>
+      <c r="B69" t="s">
+        <v>340</v>
+      </c>
+      <c r="C69" t="s">
+        <v>339</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>504</v>
+      </c>
+      <c r="F69" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>341</v>
+      </c>
+      <c r="B70" t="s">
+        <v>340</v>
+      </c>
+      <c r="C70" t="s">
+        <v>339</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70" t="s">
+        <v>505</v>
+      </c>
+      <c r="F70" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>341</v>
+      </c>
+      <c r="B71" t="s">
+        <v>340</v>
+      </c>
+      <c r="C71" t="s">
+        <v>339</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71" t="s">
+        <v>506</v>
+      </c>
+      <c r="F71" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>341</v>
+      </c>
+      <c r="B72" t="s">
+        <v>340</v>
+      </c>
+      <c r="C72" t="s">
+        <v>339</v>
+      </c>
+      <c r="D72">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>507</v>
+      </c>
+      <c r="F72" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>341</v>
+      </c>
+      <c r="B73" t="s">
+        <v>340</v>
+      </c>
+      <c r="C73" t="s">
+        <v>339</v>
+      </c>
+      <c r="D73">
+        <v>7</v>
+      </c>
+      <c r="E73" t="s">
+        <v>508</v>
+      </c>
+      <c r="F73" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>341</v>
+      </c>
+      <c r="B74" t="s">
+        <v>340</v>
+      </c>
+      <c r="C74" t="s">
+        <v>339</v>
+      </c>
+      <c r="D74">
+        <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>509</v>
+      </c>
+      <c r="F74" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>341</v>
+      </c>
+      <c r="B75" t="s">
+        <v>340</v>
+      </c>
+      <c r="C75" t="s">
+        <v>339</v>
+      </c>
+      <c r="D75">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>510</v>
+      </c>
+      <c r="F75" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>308</v>
+      </c>
+      <c r="B76" t="s">
+        <v>307</v>
+      </c>
+      <c r="C76" t="s">
+        <v>306</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
+        <v>511</v>
+      </c>
+      <c r="F76" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>308</v>
+      </c>
+      <c r="B77" t="s">
+        <v>307</v>
+      </c>
+      <c r="C77" t="s">
+        <v>306</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77" t="s">
+        <v>512</v>
+      </c>
+      <c r="F77" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>308</v>
+      </c>
+      <c r="B78" t="s">
+        <v>307</v>
+      </c>
+      <c r="C78" t="s">
+        <v>306</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+      <c r="E78" t="s">
+        <v>513</v>
+      </c>
+      <c r="F78" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>308</v>
+      </c>
+      <c r="B79" t="s">
+        <v>307</v>
+      </c>
+      <c r="C79" t="s">
+        <v>306</v>
+      </c>
+      <c r="D79">
+        <v>4</v>
+      </c>
+      <c r="E79" t="s">
+        <v>514</v>
+      </c>
+      <c r="F79" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>308</v>
+      </c>
+      <c r="B80" t="s">
+        <v>307</v>
+      </c>
+      <c r="C80" t="s">
+        <v>306</v>
+      </c>
+      <c r="D80">
+        <v>5</v>
+      </c>
+      <c r="E80" t="s">
+        <v>515</v>
+      </c>
+      <c r="F80" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>308</v>
+      </c>
+      <c r="B81" t="s">
+        <v>307</v>
+      </c>
+      <c r="C81" t="s">
+        <v>306</v>
+      </c>
+      <c r="D81">
+        <v>6</v>
+      </c>
+      <c r="E81" t="s">
+        <v>516</v>
+      </c>
+      <c r="F81" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>308</v>
+      </c>
+      <c r="B82" t="s">
+        <v>307</v>
+      </c>
+      <c r="C82" t="s">
+        <v>306</v>
+      </c>
+      <c r="D82">
+        <v>7</v>
+      </c>
+      <c r="E82" t="s">
+        <v>517</v>
+      </c>
+      <c r="F82" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>308</v>
+      </c>
+      <c r="B83" t="s">
+        <v>307</v>
+      </c>
+      <c r="C83" t="s">
+        <v>306</v>
+      </c>
+      <c r="D83">
+        <v>8</v>
+      </c>
+      <c r="E83" t="s">
+        <v>518</v>
+      </c>
+      <c r="F83" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>308</v>
+      </c>
+      <c r="B84" t="s">
+        <v>307</v>
+      </c>
+      <c r="C84" t="s">
+        <v>306</v>
+      </c>
+      <c r="D84">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>519</v>
+      </c>
+      <c r="F84" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>308</v>
+      </c>
+      <c r="B85" t="s">
+        <v>307</v>
+      </c>
+      <c r="C85" t="s">
+        <v>306</v>
+      </c>
+      <c r="D85">
+        <v>10</v>
+      </c>
+      <c r="E85" t="s">
+        <v>520</v>
+      </c>
+      <c r="F85" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>308</v>
+      </c>
+      <c r="B86" t="s">
+        <v>307</v>
+      </c>
+      <c r="C86" t="s">
+        <v>306</v>
+      </c>
+      <c r="D86">
+        <v>11</v>
+      </c>
+      <c r="E86" t="s">
+        <v>521</v>
+      </c>
+      <c r="F86" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>308</v>
+      </c>
+      <c r="B87" t="s">
+        <v>307</v>
+      </c>
+      <c r="C87" t="s">
+        <v>306</v>
+      </c>
+      <c r="D87">
+        <v>12</v>
+      </c>
+      <c r="E87" t="s">
+        <v>522</v>
+      </c>
+      <c r="F87" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>308</v>
+      </c>
+      <c r="B88" t="s">
+        <v>307</v>
+      </c>
+      <c r="C88" t="s">
+        <v>306</v>
+      </c>
+      <c r="D88">
+        <v>13</v>
+      </c>
+      <c r="E88" t="s">
+        <v>523</v>
+      </c>
+      <c r="F88" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>308</v>
+      </c>
+      <c r="B89" t="s">
+        <v>307</v>
+      </c>
+      <c r="C89" t="s">
+        <v>306</v>
+      </c>
+      <c r="D89">
+        <v>14</v>
+      </c>
+      <c r="E89" t="s">
+        <v>524</v>
+      </c>
+      <c r="F89" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>308</v>
+      </c>
+      <c r="B90" t="s">
+        <v>307</v>
+      </c>
+      <c r="C90" t="s">
+        <v>306</v>
+      </c>
+      <c r="D90">
+        <v>15</v>
+      </c>
+      <c r="E90" t="s">
+        <v>525</v>
+      </c>
+      <c r="F90" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>308</v>
+      </c>
+      <c r="B91" t="s">
+        <v>307</v>
+      </c>
+      <c r="C91" t="s">
+        <v>306</v>
+      </c>
+      <c r="D91">
+        <v>16</v>
+      </c>
+      <c r="E91" t="s">
+        <v>526</v>
+      </c>
+      <c r="F91" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>308</v>
+      </c>
+      <c r="B92" t="s">
+        <v>307</v>
+      </c>
+      <c r="C92" t="s">
+        <v>306</v>
+      </c>
+      <c r="D92">
+        <v>17</v>
+      </c>
+      <c r="E92" t="s">
+        <v>527</v>
+      </c>
+      <c r="F92" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>308</v>
+      </c>
+      <c r="B93" t="s">
+        <v>307</v>
+      </c>
+      <c r="C93" t="s">
+        <v>306</v>
+      </c>
+      <c r="D93">
+        <v>18</v>
+      </c>
+      <c r="E93" t="s">
+        <v>528</v>
+      </c>
+      <c r="F93" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>308</v>
+      </c>
+      <c r="B94" t="s">
+        <v>307</v>
+      </c>
+      <c r="C94" t="s">
+        <v>306</v>
+      </c>
+      <c r="D94">
+        <v>19</v>
+      </c>
+      <c r="E94" t="s">
+        <v>529</v>
+      </c>
+      <c r="F94" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>308</v>
+      </c>
+      <c r="B95" t="s">
+        <v>307</v>
+      </c>
+      <c r="C95" t="s">
+        <v>306</v>
+      </c>
+      <c r="D95">
+        <v>20</v>
+      </c>
+      <c r="E95" t="s">
+        <v>530</v>
+      </c>
+      <c r="F95" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>308</v>
+      </c>
+      <c r="B96" t="s">
+        <v>307</v>
+      </c>
+      <c r="C96" t="s">
+        <v>306</v>
+      </c>
+      <c r="D96">
+        <v>21</v>
+      </c>
+      <c r="E96" t="s">
+        <v>531</v>
+      </c>
+      <c r="F96" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>308</v>
+      </c>
+      <c r="B97" t="s">
+        <v>307</v>
+      </c>
+      <c r="C97" t="s">
+        <v>306</v>
+      </c>
+      <c r="D97">
+        <v>22</v>
+      </c>
+      <c r="E97" t="s">
+        <v>532</v>
+      </c>
+      <c r="F97" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>308</v>
+      </c>
+      <c r="B98" t="s">
+        <v>307</v>
+      </c>
+      <c r="C98" t="s">
+        <v>306</v>
+      </c>
+      <c r="D98">
+        <v>23</v>
+      </c>
+      <c r="E98" t="s">
+        <v>533</v>
+      </c>
+      <c r="F98" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>308</v>
+      </c>
+      <c r="B99" t="s">
+        <v>307</v>
+      </c>
+      <c r="C99" t="s">
+        <v>306</v>
+      </c>
+      <c r="D99">
+        <v>24</v>
+      </c>
+      <c r="E99" t="s">
+        <v>534</v>
+      </c>
+      <c r="F99" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>308</v>
+      </c>
+      <c r="B100" t="s">
+        <v>307</v>
+      </c>
+      <c r="C100" t="s">
+        <v>306</v>
+      </c>
+      <c r="D100">
+        <v>25</v>
+      </c>
+      <c r="E100" t="s">
+        <v>535</v>
+      </c>
+      <c r="F100" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>308</v>
+      </c>
+      <c r="B101" t="s">
+        <v>307</v>
+      </c>
+      <c r="C101" t="s">
+        <v>306</v>
+      </c>
+      <c r="D101">
+        <v>26</v>
+      </c>
+      <c r="E101" t="s">
+        <v>536</v>
+      </c>
+      <c r="F101" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>308</v>
+      </c>
+      <c r="B102" t="s">
+        <v>307</v>
+      </c>
+      <c r="C102" t="s">
+        <v>306</v>
+      </c>
+      <c r="D102">
+        <v>27</v>
+      </c>
+      <c r="E102" t="s">
+        <v>537</v>
+      </c>
+      <c r="F102" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>308</v>
+      </c>
+      <c r="B103" t="s">
+        <v>307</v>
+      </c>
+      <c r="C103" t="s">
+        <v>306</v>
+      </c>
+      <c r="D103">
+        <v>28</v>
+      </c>
+      <c r="E103" t="s">
+        <v>538</v>
+      </c>
+      <c r="F103" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>308</v>
+      </c>
+      <c r="B104" t="s">
+        <v>307</v>
+      </c>
+      <c r="C104" t="s">
+        <v>306</v>
+      </c>
+      <c r="D104">
+        <v>29</v>
+      </c>
+      <c r="E104" t="s">
+        <v>539</v>
+      </c>
+      <c r="F104" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>308</v>
+      </c>
+      <c r="B105" t="s">
+        <v>307</v>
+      </c>
+      <c r="C105" t="s">
+        <v>306</v>
+      </c>
+      <c r="D105">
+        <v>30</v>
+      </c>
+      <c r="E105" t="s">
+        <v>540</v>
+      </c>
+      <c r="F105" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>298</v>
+      </c>
+      <c r="B106" t="s">
+        <v>297</v>
+      </c>
+      <c r="C106" t="s">
+        <v>296</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106" t="s">
+        <v>541</v>
+      </c>
+      <c r="F106" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>298</v>
+      </c>
+      <c r="B107" t="s">
+        <v>297</v>
+      </c>
+      <c r="C107" t="s">
+        <v>296</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+      <c r="E107" t="s">
+        <v>542</v>
+      </c>
+      <c r="F107" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>298</v>
+      </c>
+      <c r="B108" t="s">
+        <v>297</v>
+      </c>
+      <c r="C108" t="s">
+        <v>296</v>
+      </c>
+      <c r="D108">
+        <v>3</v>
+      </c>
+      <c r="E108" t="s">
+        <v>543</v>
+      </c>
+      <c r="F108" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>298</v>
+      </c>
+      <c r="B109" t="s">
+        <v>297</v>
+      </c>
+      <c r="C109" t="s">
+        <v>296</v>
+      </c>
+      <c r="D109">
+        <v>4</v>
+      </c>
+      <c r="E109" t="s">
+        <v>544</v>
+      </c>
+      <c r="F109" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>298</v>
+      </c>
+      <c r="B110" t="s">
+        <v>297</v>
+      </c>
+      <c r="C110" t="s">
+        <v>296</v>
+      </c>
+      <c r="D110">
+        <v>5</v>
+      </c>
+      <c r="E110" t="s">
+        <v>545</v>
+      </c>
+      <c r="F110" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>298</v>
+      </c>
+      <c r="B111" t="s">
+        <v>297</v>
+      </c>
+      <c r="C111" t="s">
+        <v>296</v>
+      </c>
+      <c r="D111">
+        <v>6</v>
+      </c>
+      <c r="E111" t="s">
+        <v>546</v>
+      </c>
+      <c r="F111" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>298</v>
+      </c>
+      <c r="B112" t="s">
+        <v>297</v>
+      </c>
+      <c r="C112" t="s">
+        <v>296</v>
+      </c>
+      <c r="D112">
+        <v>7</v>
+      </c>
+      <c r="E112" t="s">
+        <v>547</v>
+      </c>
+      <c r="F112" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>